<commit_message>
feat: introduce async course fetcher with DB, OCR, notifications and charts
- Add `sqltools.py` for PostgreSQL operations (asyncpg, schema init, UPSERT)
- Add `notifiers.py` with multi-channel support:
  - short_msg (Twilio SMS)
  - send_mail (SMTP email with attachments)
  - send_line (LINE Bot messaging)

- Generate interactive charts (`courses_bar.html`, `courses_pie.html`) with Plotly
- Export Excel file `schedule.xlsx` for user records
- Store analysis results and screenshots under `resaults/` for showcase

- Optimize and finalize main script `asyncio-course-fetcher.py`
- Improved logging for full workflow traceability
- Adjusted `config.yaml` to remove `headless` option (improves OCR recognition)

- Extend `.env` with full configuration items (DB, Twilio, SMTP, LINE, etc.)
- Update `pyproject.toml` with corrected project description

- Rewrite and complete `README.md` with full usage guide and architecture
- Add "Showcase" section with results screenshot
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1173,7 +1173,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>空堂 - Free Period</t>
+          <t>嵌入式微算機系統 - Embeded Microcomputer System</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>空堂 - Free Period</t>
+          <t>嵌入式微算機系統 - Embeded Microcomputer System</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>空堂 - Free Period</t>
+          <t>嵌入式微算機系統 - Embeded Microcomputer System</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>